<commit_message>
66 page complete thesis. submitted this. have to spell check and do plag modifications. add an appendix also..
</commit_message>
<xml_diff>
--- a/figures-bharath/ResultsReport.xlsx
+++ b/figures-bharath/ResultsReport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="38">
   <si>
     <t>Camera dataset</t>
   </si>
@@ -128,6 +128,12 @@
   <si>
     <t>INIT</t>
   </si>
+  <si>
+    <t>finalMix-opt</t>
+  </si>
+  <si>
+    <t>finalMix-noisy</t>
+  </si>
 </sst>
 </file>
 
@@ -196,8 +202,130 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="313">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -409,7 +537,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="313">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -505,6 +633,67 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -600,6 +789,67 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,7 +938,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SIM</c:v>
+                  <c:v>INIT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -718,13 +968,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.12</c:v>
+                  <c:v>6.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.24</c:v>
+                  <c:v>3.11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.52</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -739,7 +989,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SIM+ADDPREF</c:v>
+                  <c:v>ADD</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -769,13 +1019,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.34</c:v>
+                  <c:v>6.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.71</c:v>
+                  <c:v>3.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.42</c:v>
+                  <c:v>1.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HIST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Q1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Q3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Q5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -873,7 +1174,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000"/>
+            <a:defRPr sz="2500"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1278,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN72"/>
+  <dimension ref="A1:AN88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R33" workbookViewId="0">
-      <selection activeCell="AH66" sqref="AH66"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71:N71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1326,16 +1627,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4">
-        <v>5.12</v>
+        <v>6.31</v>
       </c>
       <c r="C3" s="4">
-        <v>2.2400000000000002</v>
+        <v>3.11</v>
       </c>
       <c r="D3" s="4">
-        <v>1.52</v>
+        <v>1.64</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -1343,30 +1644,30 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4">
-        <v>4.34</v>
+        <v>6.12</v>
       </c>
       <c r="C4" s="4">
-        <v>1.71</v>
+        <v>3.06</v>
       </c>
       <c r="D4" s="4">
-        <v>1.42</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="6">
-        <v>6.11</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2.91</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1.31</v>
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>6.01</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.02</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.65</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1416,6 +1717,151 @@
         <v>1.88</v>
       </c>
     </row>
+    <row r="21" spans="24:27">
+      <c r="X21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="24:27" ht="30">
+      <c r="X22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="24:27">
+      <c r="X23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>4.08</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="24:27">
+      <c r="X24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y24" s="4">
+        <v>8.81</v>
+      </c>
+      <c r="Z24" s="4">
+        <v>3.71</v>
+      </c>
+      <c r="AA24" s="4">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="25" spans="24:27">
+      <c r="X25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y25" s="4">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="Z25" s="4">
+        <v>3.68</v>
+      </c>
+      <c r="AA25" s="4">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="26" spans="24:27">
+      <c r="X26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y26" s="6">
+        <v>8.51</v>
+      </c>
+      <c r="Z26" s="6">
+        <v>3.51</v>
+      </c>
+      <c r="AA26" s="6">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="28" spans="24:27">
+      <c r="X28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="24:27">
+      <c r="X29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>6.62</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="30" spans="24:27">
+      <c r="X30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y30" s="4">
+        <v>6.12</v>
+      </c>
+      <c r="Z30" s="4">
+        <v>2.91</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="31" spans="24:27">
+      <c r="X31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y31" s="4">
+        <v>6.02</v>
+      </c>
+      <c r="Z31" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="AA31" s="4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="32" spans="24:27">
+      <c r="X32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y32" s="4">
+        <v>6.41</v>
+      </c>
+      <c r="Z32" s="4">
+        <v>2.96</v>
+      </c>
+      <c r="AA32" s="4">
+        <v>1.66</v>
+      </c>
+    </row>
     <row r="36" spans="1:40">
       <c r="A36" t="s">
         <v>9</v>
@@ -1784,37 +2230,37 @@
     </row>
     <row r="41" spans="1:40">
       <c r="B41">
-        <f>((B38-B39)/B38)*100</f>
-        <v>15.092290988056464</v>
+        <f>((B38-B40)/B38)*100</f>
+        <v>25.95005428881651</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:D41" si="0">((C38-C39)/C38)*100</f>
-        <v>23.52941176470588</v>
+        <f t="shared" ref="C41:D41" si="0">((C38-C40)/C38)*100</f>
+        <v>26.225490196078439</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>29.353233830845767</v>
+        <v>31.343283582089548</v>
       </c>
       <c r="E41">
         <f>AVERAGE(B41:D41)</f>
-        <v>22.658312194536038</v>
+        <v>27.839609355661498</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41">
-        <f>((G38-G40)/G38)*100</f>
-        <v>35.72204125950055</v>
+        <f>((G38-G39)/G38)*100</f>
+        <v>30.293159609120529</v>
       </c>
       <c r="H41">
-        <f t="shared" ref="H41:I41" si="1">((H38-H40)/H38)*100</f>
-        <v>33.333333333333329</v>
+        <f t="shared" ref="H41:I41" si="1">((H38-H39)/H38)*100</f>
+        <v>31.372549019607849</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>32.338308457711427</v>
+        <v>31.840796019900488</v>
       </c>
       <c r="J41">
         <f>AVERAGE(G41:I41)</f>
-        <v>33.797894350181771</v>
+        <v>31.168834882876286</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>25</v>
@@ -1829,20 +2275,20 @@
         <v>1.42</v>
       </c>
       <c r="AA41">
-        <f>((AA38-AA40)/AA38)*100</f>
-        <v>38.979370249728561</v>
+        <f>((AA38-AA39)/AA38)*100</f>
+        <v>30.184581976112927</v>
       </c>
       <c r="AB41">
-        <f t="shared" ref="AB41:AC41" si="2">((AB38-AB40)/AB38)*100</f>
-        <v>44.117647058823536</v>
+        <f t="shared" ref="AB41:AC41" si="2">((AB38-AB39)/AB38)*100</f>
+        <v>38.480392156862756</v>
       </c>
       <c r="AC41">
         <f t="shared" si="2"/>
-        <v>37.810945273631837</v>
+        <v>29.353233830845767</v>
       </c>
       <c r="AD41">
         <f>AVERAGE(AA41:AC41)</f>
-        <v>40.302654194061311</v>
+        <v>32.672735987940484</v>
       </c>
       <c r="AM41" s="5">
         <v>1.4</v>
@@ -1862,6 +2308,22 @@
       <c r="D42" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L42">
+        <f>((L38-L40)/L38)*100</f>
+        <v>23.127035830618901</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ref="M42:N42" si="3">((M38-M40)/M38)*100</f>
+        <v>18.627450980392162</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="3"/>
+        <v>24.875621890547254</v>
+      </c>
+      <c r="O42">
+        <f>AVERAGE(L42:N42)</f>
+        <v>22.210036233852772</v>
+      </c>
       <c r="AM42" s="5">
         <v>1.5</v>
       </c>
@@ -2134,12 +2596,28 @@
         <v>1.7</v>
       </c>
       <c r="AM45" s="5">
-        <f t="shared" ref="AM45:AM57" si="3">AM44+0.1</f>
+        <f t="shared" ref="AM45:AM57" si="4">AM44+0.1</f>
         <v>1.8000000000000003</v>
       </c>
       <c r="AN45" s="6"/>
     </row>
     <row r="46" spans="1:40">
+      <c r="B46">
+        <f>((B43-B45)/B43)*100</f>
+        <v>11.933534743202417</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46" si="5">((C43-C45)/C43)*100</f>
+        <v>9.3548387096774199</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ref="D46" si="6">((D43-D45)/D43)*100</f>
+        <v>12.716763005780345</v>
+      </c>
+      <c r="E46">
+        <f>AVERAGE(B46:D46)</f>
+        <v>11.335045486220061</v>
+      </c>
       <c r="F46" s="5" t="s">
         <v>14</v>
       </c>
@@ -2177,16 +2655,29 @@
         <v>1.31</v>
       </c>
       <c r="AM46" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9000000000000004</v>
       </c>
       <c r="AN46" s="6"/>
     </row>
     <row r="47" spans="1:40">
       <c r="F47" s="5"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="G47">
+        <f>((G44-G46)/G44)*100</f>
+        <v>15.105740181268882</v>
+      </c>
+      <c r="H47">
+        <f t="shared" ref="H47:I47" si="7">((H44-H46)/H44)*100</f>
+        <v>6.4516129032258114</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="7"/>
+        <v>6.9364161849710921</v>
+      </c>
+      <c r="J47">
+        <f>AVERAGE(G47:I47)</f>
+        <v>9.4979230898219296</v>
+      </c>
       <c r="K47" s="5" t="s">
         <v>25</v>
       </c>
@@ -2199,8 +2690,24 @@
       <c r="N47" s="6">
         <v>1.31</v>
       </c>
+      <c r="AA47">
+        <f>((AA44-AA45)/AA44)*100</f>
+        <v>30.513595166163149</v>
+      </c>
+      <c r="AB47">
+        <f t="shared" ref="AB47:AC47" si="8">((AB44-AB45)/AB44)*100</f>
+        <v>35.483870967741936</v>
+      </c>
+      <c r="AC47">
+        <f t="shared" si="8"/>
+        <v>23.699421965317917</v>
+      </c>
+      <c r="AD47">
+        <f>AVERAGE(AA47:AC47)</f>
+        <v>29.898962699741002</v>
+      </c>
       <c r="AM47" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.0000000000000004</v>
       </c>
       <c r="AN47" s="6">
@@ -2208,8 +2715,24 @@
       </c>
     </row>
     <row r="48" spans="1:40">
+      <c r="L48">
+        <f>((L44-L46)/L44)*100</f>
+        <v>3.0211480362537788</v>
+      </c>
+      <c r="M48">
+        <f t="shared" ref="M48:N48" si="9">((M44-M46)/M44)*100</f>
+        <v>3.2258064516129057</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="9"/>
+        <v>12.716763005780345</v>
+      </c>
+      <c r="O48">
+        <f>AVERAGE(L48:N48)</f>
+        <v>6.3212391645490102</v>
+      </c>
       <c r="AM48" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.1000000000000005</v>
       </c>
       <c r="AN48" s="6"/>
@@ -2225,7 +2748,7 @@
         <v>27</v>
       </c>
       <c r="AM49" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2000000000000006</v>
       </c>
       <c r="AN49" s="6"/>
@@ -2235,7 +2758,7 @@
         <v>16</v>
       </c>
       <c r="AM50" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.3000000000000007</v>
       </c>
       <c r="AN50" s="6"/>
@@ -2248,35 +2771,35 @@
         <v>33</v>
       </c>
       <c r="AM51" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4000000000000008</v>
       </c>
       <c r="AN51" s="6"/>
     </row>
     <row r="52" spans="1:40">
       <c r="AM52" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5000000000000009</v>
       </c>
       <c r="AN52" s="6"/>
     </row>
     <row r="53" spans="1:40">
       <c r="AM53" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.600000000000001</v>
       </c>
       <c r="AN53" s="6"/>
     </row>
     <row r="54" spans="1:40">
       <c r="AM54" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7000000000000011</v>
       </c>
       <c r="AN54" s="6"/>
     </row>
     <row r="55" spans="1:40">
       <c r="AM55" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8000000000000012</v>
       </c>
       <c r="AN55" s="6"/>
@@ -2286,14 +2809,14 @@
         <v>28</v>
       </c>
       <c r="AM56" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9000000000000012</v>
       </c>
       <c r="AN56" s="6"/>
     </row>
     <row r="57" spans="1:40">
       <c r="AM57" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0000000000000013</v>
       </c>
       <c r="AN57" s="6"/>
@@ -2327,7 +2850,7 @@
         <v>20</v>
       </c>
       <c r="AF59" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:40" ht="30">
@@ -2576,7 +3099,7 @@
         <v>1.56</v>
       </c>
       <c r="AF62" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="AG62" s="4">
         <v>9.3000000000000007</v>
@@ -2639,10 +3162,39 @@
       </c>
     </row>
     <row r="64" spans="1:40">
+      <c r="B64">
+        <f>((B61-B62)/B61)*100</f>
+        <v>21.739130434782609</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ref="C64:D64" si="10">((C61-C62)/C61)*100</f>
+        <v>29.327902240325866</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="10"/>
+        <v>37.448559670781897</v>
+      </c>
+      <c r="E64">
+        <f>AVERAGE(B64:D64)</f>
+        <v>29.505197448630128</v>
+      </c>
       <c r="F64" s="5"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
+      <c r="G64">
+        <f>((G61-G63)/G61)*100</f>
+        <v>36.038647342995169</v>
+      </c>
+      <c r="H64">
+        <f t="shared" ref="H64" si="11">((H61-H63)/H61)*100</f>
+        <v>34.419551934826877</v>
+      </c>
+      <c r="I64">
+        <f t="shared" ref="I64" si="12">((I61-I63)/I61)*100</f>
+        <v>37.860082304526756</v>
+      </c>
+      <c r="J64">
+        <f>AVERAGE(G64:I64)</f>
+        <v>36.106093860782934</v>
+      </c>
       <c r="K64" s="5" t="s">
         <v>25</v>
       </c>
@@ -2654,6 +3206,22 @@
       </c>
       <c r="N64" s="6">
         <v>1.51</v>
+      </c>
+      <c r="AA64">
+        <f>((AA61-AA62)/AA61)*100</f>
+        <v>30.241545893719806</v>
+      </c>
+      <c r="AB64">
+        <f t="shared" ref="AB64:AC64" si="13">((AB61-AB62)/AB61)*100</f>
+        <v>46.843177189409374</v>
+      </c>
+      <c r="AC64">
+        <f t="shared" si="13"/>
+        <v>35.802469135802475</v>
+      </c>
+      <c r="AD64">
+        <f>AVERAGE(AA64:AC64)</f>
+        <v>37.629064072977222</v>
       </c>
     </row>
     <row r="65" spans="1:35">
@@ -2669,6 +3237,22 @@
       <c r="D65" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L65">
+        <f>((L61-L63)/L61)*100</f>
+        <v>29.178743961352655</v>
+      </c>
+      <c r="M65">
+        <f t="shared" ref="M65:N65" si="14">((M61-M63)/M61)*100</f>
+        <v>29.735234215885946</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="14"/>
+        <v>33.744855967078195</v>
+      </c>
+      <c r="O65">
+        <f>AVERAGE(L65:N65)</f>
+        <v>30.886278048105599</v>
+      </c>
     </row>
     <row r="66" spans="1:35">
       <c r="A66" s="2" t="s">
@@ -2916,7 +3500,7 @@
         <v>1.52</v>
       </c>
       <c r="AF68" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="AG68" s="4">
         <v>6.31</v>
@@ -2929,6 +3513,22 @@
       </c>
     </row>
     <row r="69" spans="1:35">
+      <c r="B69">
+        <f>((B66-B68)/B66)*100</f>
+        <v>13.956834532374096</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ref="C69:D69" si="15">((C66-C68)/C66)*100</f>
+        <v>31.578947368421051</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="15"/>
+        <v>29.651162790697676</v>
+      </c>
+      <c r="E69">
+        <f>AVERAGE(B69:D69)</f>
+        <v>25.062314897164271</v>
+      </c>
       <c r="F69" s="5" t="s">
         <v>14</v>
       </c>
@@ -2968,9 +3568,22 @@
     </row>
     <row r="70" spans="1:35">
       <c r="F70" s="5"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
+      <c r="G70">
+        <f>((G67-G69)/G67)*100</f>
+        <v>17.841726618705039</v>
+      </c>
+      <c r="H70">
+        <f t="shared" ref="H70" si="16">((H67-H69)/H67)*100</f>
+        <v>17.956656346749227</v>
+      </c>
+      <c r="I70">
+        <f t="shared" ref="I70" si="17">((I67-I69)/I67)*100</f>
+        <v>29.239766081871345</v>
+      </c>
+      <c r="J70">
+        <f>AVERAGE(G70:I70)</f>
+        <v>21.679383015775205</v>
+      </c>
       <c r="K70" s="5" t="s">
         <v>25</v>
       </c>
@@ -2982,11 +3595,190 @@
       </c>
       <c r="N70" s="6">
         <v>1.31</v>
+      </c>
+      <c r="AA70">
+        <f>((AA67-AA68)/AA67)*100</f>
+        <v>32.086330935251809</v>
+      </c>
+      <c r="AB70">
+        <f t="shared" ref="AB70:AC70" si="18">((AB67-AB68)/AB67)*100</f>
+        <v>30.650154798761601</v>
+      </c>
+      <c r="AC70">
+        <f t="shared" si="18"/>
+        <v>11.111111111111107</v>
+      </c>
+      <c r="AD70">
+        <f>AVERAGE(AA70:AC70)</f>
+        <v>24.615865615041503</v>
+      </c>
+    </row>
+    <row r="71" spans="1:35">
+      <c r="L71">
+        <f>((L67-L69)/L67)*100</f>
+        <v>10.647482014388492</v>
+      </c>
+      <c r="M71">
+        <f t="shared" ref="M71:N71" si="19">((M67-M69)/M67)*100</f>
+        <v>6.1919504643962906</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="19"/>
+        <v>11.695906432748536</v>
+      </c>
+      <c r="O71">
+        <f>AVERAGE(L71:N71)</f>
+        <v>9.5117796371777725</v>
       </c>
     </row>
     <row r="72" spans="1:35">
       <c r="F72" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35">
+      <c r="W77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35" ht="30">
+      <c r="W78" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z78" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35">
+      <c r="W79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X79" s="3">
+        <v>10.35</v>
+      </c>
+      <c r="Y79" s="3">
+        <v>4.91</v>
+      </c>
+      <c r="Z79" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35">
+      <c r="W80" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X80" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="Y80" s="4">
+        <v>4.08</v>
+      </c>
+      <c r="Z80" s="4">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="81" spans="23:26">
+      <c r="W81" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X81" s="4">
+        <v>9.1</v>
+      </c>
+      <c r="Y81" s="4">
+        <v>3.72</v>
+      </c>
+      <c r="Z81" s="4">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="82" spans="23:26">
+      <c r="W82" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X82" s="6">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="Y82" s="6">
+        <v>3.92</v>
+      </c>
+      <c r="Z82" s="6">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="84" spans="23:26">
+      <c r="W84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z84" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="23:26">
+      <c r="W85" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X85" s="3">
+        <v>6.95</v>
+      </c>
+      <c r="Y85" s="3">
+        <v>3.23</v>
+      </c>
+      <c r="Z85" s="3">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="86" spans="23:26">
+      <c r="W86" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X86" s="4">
+        <v>6.31</v>
+      </c>
+      <c r="Y86" s="4">
+        <v>3.11</v>
+      </c>
+      <c r="Z86" s="4">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="87" spans="23:26">
+      <c r="W87" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X87" s="4">
+        <v>6.12</v>
+      </c>
+      <c r="Y87" s="4">
+        <v>3.06</v>
+      </c>
+      <c r="Z87" s="4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="88" spans="23:26">
+      <c r="W88" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="X88" s="4">
+        <v>6.01</v>
+      </c>
+      <c r="Y88" s="4">
+        <v>3.02</v>
+      </c>
+      <c r="Z88" s="4">
+        <v>1.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>